<commit_message>
Fix state view colours and school attendance status.
</commit_message>
<xml_diff>
--- a/dashboard_loader/indigenous_school_attendance_uploader/indigenous_school_attendance.xlsx
+++ b/dashboard_loader/indigenous_school_attendance_uploader/indigenous_school_attendance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -80,7 +80,7 @@
     <t xml:space="preserve">Status</t>
   </si>
   <si>
-    <t xml:space="preserve">On track</t>
+    <t xml:space="preserve">Not on track</t>
   </si>
   <si>
     <t xml:space="preserve">Updated</t>
@@ -362,8 +362,8 @@
   </sheetPr>
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -606,8 +606,8 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>